<commit_message>
Updated testcases for conf final submission - Iter 1.0
</commit_message>
<xml_diff>
--- a/Testcases_Part1.xlsx
+++ b/Testcases_Part1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PREETHI\Coursewise_Documents\Sem_7\BTP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Academics\Semester7\BTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5857F2C-7360-4B60-9B4E-48529AAC0C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C189E00E-D708-49AA-8181-9A34D74FB7F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{82200626-AD99-4240-B52B-FF0FA02B1A32}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{82200626-AD99-4240-B52B-FF0FA02B1A32}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="27">
   <si>
     <t>Arm</t>
   </si>
@@ -99,13 +99,22 @@
   </si>
   <si>
     <t>Arm 2, Attr 2 varies from 0.5 to 0.7</t>
+  </si>
+  <si>
+    <t>Delta_i/2</t>
+  </si>
+  <si>
+    <t>Detecting feasibility</t>
+  </si>
+  <si>
+    <t>Detecting overall mean</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,16 +122,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -222,13 +264,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -237,6 +291,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,358 +614,360 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D6CE0F-EB49-4DFC-B767-40CF11993C49}">
-  <dimension ref="D3:S16"/>
+  <dimension ref="D3:S25"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="4:19" x14ac:dyDescent="0.3">
       <c r="E3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="4:19" x14ac:dyDescent="0.35">
-      <c r="E6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="8" t="s">
+      <c r="L3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="E6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="L6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="8" t="s">
+      <c r="M6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="N6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="O6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="P6" s="8" t="s">
+      <c r="O6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="Q6" s="8" t="s">
+      <c r="Q6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R6" s="8" t="s">
+      <c r="R6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="S6" s="9" t="s">
+      <c r="S6" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="4:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>1</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="17">
         <v>0.5</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="11">
         <v>0.6</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="11">
         <v>0.7</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="11">
         <v>0.7</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="11">
         <v>0.8</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="13">
         <f>SUM(F7:J7)/5</f>
         <v>0.65999999999999992</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7">
         <v>0.3</v>
       </c>
-      <c r="M7" s="1" t="b">
+      <c r="M7" t="b">
         <f>MIN(F7:J7)&gt;L7</f>
         <v>1</v>
       </c>
-      <c r="N7" s="1" t="b">
+      <c r="N7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="O7" s="1">
-        <f>IF(OR($N$7:$N$11)=0,2,O10)</f>
-        <v>3.5000000000000087E-2</v>
-      </c>
-      <c r="P7" s="1">
+      <c r="O7">
+        <f>IF(OR($N$7:$N$11)=0,2,O8)</f>
+        <v>5.9999999999999942E-2</v>
+      </c>
+      <c r="P7">
         <f>ABS(MIN(F7:J7)-L7)</f>
         <v>0.2</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="Q7">
         <f>(M7*N7/O7)^2</f>
         <v>0</v>
       </c>
-      <c r="R7" s="1">
+      <c r="R7">
         <f>((1-M7)*(1-N7)/P7)^2</f>
         <v>0</v>
       </c>
-      <c r="S7" s="3">
+      <c r="S7" s="2">
         <f>((1-M7)*N7/MAX(O7, P7))^2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="4:19" x14ac:dyDescent="0.35">
-      <c r="E8" s="5">
+    <row r="8" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="4">
         <v>2</v>
       </c>
-      <c r="F8" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="G8" s="1">
+      <c r="F8" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="G8" s="11">
         <v>0.2</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="11">
         <v>0.5</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="11">
         <v>0.7</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="11">
         <v>0.8</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="14">
         <f t="shared" ref="K8:K11" si="0">SUM(F8:J8)/5</f>
-        <v>0.61999999999999988</v>
-      </c>
-      <c r="L8" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="L8">
         <v>0.3</v>
       </c>
-      <c r="M8" s="1" t="b">
+      <c r="M8" t="b">
         <f t="shared" ref="M8:M11" si="1">MIN(F8:J8)&gt;L8</f>
         <v>0</v>
       </c>
-      <c r="N8" s="1" t="b">
+      <c r="N8" t="b">
         <f>K8&lt;$K$7</f>
         <v>1</v>
       </c>
-      <c r="O8" s="1">
+      <c r="O8">
         <f>ABS(K8-$K$7)/2</f>
-        <v>2.0000000000000018E-2</v>
-      </c>
-      <c r="P8" s="1">
+        <v>5.9999999999999942E-2</v>
+      </c>
+      <c r="P8">
         <f t="shared" ref="P8:P11" si="2">ABS(MIN(F8:J8)-L8)</f>
         <v>9.9999999999999978E-2</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="Q8">
         <f t="shared" ref="Q8:Q11" si="3">(M8*N8/O8)^2</f>
         <v>0</v>
       </c>
-      <c r="R8" s="1">
+      <c r="R8">
         <f t="shared" ref="R8:R11" si="4">((1-M8)*(1-N8)/P8)^2</f>
         <v>0</v>
       </c>
-      <c r="S8" s="3">
+      <c r="S8" s="2">
         <f t="shared" ref="S8:S11" si="5">((1-M8)*N8/MAX(O8, P8))^2</f>
         <v>100.00000000000003</v>
       </c>
     </row>
-    <row r="9" spans="4:19" x14ac:dyDescent="0.35">
-      <c r="E9" s="5">
+    <row r="9" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="E9" s="4">
         <v>3</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="11">
         <v>0.15</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="11">
         <v>0.7</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="11">
         <v>0.8</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="11">
         <v>0.9</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="11">
         <v>0.9</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="14">
         <f t="shared" si="0"/>
         <v>0.69</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9">
         <v>0.3</v>
       </c>
-      <c r="M9" s="1" t="b">
+      <c r="M9" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N9" s="1" t="b">
+      <c r="N9" t="b">
         <f t="shared" ref="N9:N11" si="6">K9&lt;$K$7</f>
         <v>0</v>
       </c>
-      <c r="O9" s="1">
+      <c r="O9">
         <f t="shared" ref="O9:O11" si="7">ABS(K9-$K$7)/2</f>
         <v>1.5000000000000013E-2</v>
       </c>
-      <c r="P9" s="1">
+      <c r="P9">
         <f t="shared" si="2"/>
         <v>0.15</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="Q9">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R9" s="1">
+      <c r="R9">
         <f t="shared" si="4"/>
         <v>44.44444444444445</v>
       </c>
-      <c r="S9" s="3">
+      <c r="S9" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="4:19" x14ac:dyDescent="0.35">
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="5">
+    <row r="10" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="E10" s="4">
         <v>4</v>
       </c>
-      <c r="F10" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="G10" s="1">
+      <c r="F10" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="G10" s="11">
+        <v>0.7</v>
+      </c>
+      <c r="H10" s="11">
         <v>0.9</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="11">
         <v>0.9</v>
       </c>
-      <c r="I10" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="J10" s="1">
+      <c r="J10" s="11">
         <v>0.8</v>
       </c>
-      <c r="K10" s="1">
-        <f t="shared" si="0"/>
-        <v>0.73000000000000009</v>
-      </c>
-      <c r="L10" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="M10" s="1" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N10" s="1" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="O10" s="1">
-        <f t="shared" si="7"/>
-        <v>3.5000000000000087E-2</v>
-      </c>
-      <c r="P10" s="1">
-        <f t="shared" si="2"/>
-        <v>0.15</v>
-      </c>
-      <c r="Q10" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="R10" s="1">
-        <f t="shared" si="4"/>
-        <v>44.44444444444445</v>
-      </c>
-      <c r="S10" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="4:19" x14ac:dyDescent="0.35">
-      <c r="E11" s="6">
-        <v>5</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0.9</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0.9</v>
-      </c>
-      <c r="I11" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="J11" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="K11" s="2">
+      <c r="K10" s="14">
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L10">
         <v>0.3</v>
       </c>
-      <c r="M11" s="2" t="b">
+      <c r="M10" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N11" s="2" t="b">
+      <c r="N10" t="b">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O11" s="2">
+      <c r="O10">
         <f t="shared" si="7"/>
         <v>2.0000000000000018E-2</v>
       </c>
-      <c r="P11" s="2">
+      <c r="P10">
+        <f t="shared" si="2"/>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="4"/>
+        <v>100.00000000000003</v>
+      </c>
+      <c r="S10" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="E11" s="5">
+        <v>5</v>
+      </c>
+      <c r="F11" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="G11" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="H11" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="I11" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="J11" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="K11" s="15">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="M11" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="1" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="1">
+        <f t="shared" si="7"/>
+        <v>2.0000000000000018E-2</v>
+      </c>
+      <c r="P11" s="1">
         <f t="shared" si="2"/>
         <v>0.19999999999999998</v>
       </c>
-      <c r="Q11" s="2">
+      <c r="Q11" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R11" s="2">
+      <c r="R11" s="1">
         <f t="shared" si="4"/>
         <v>25</v>
       </c>
-      <c r="S11" s="3">
+      <c r="S11" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="4:19" x14ac:dyDescent="0.35">
+    <row r="15" spans="4:19" x14ac:dyDescent="0.3">
       <c r="H15" t="s">
         <v>8</v>
       </c>
@@ -916,10 +981,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="4:19" x14ac:dyDescent="0.35">
+    <row r="16" spans="4:19" x14ac:dyDescent="0.3">
       <c r="H16">
         <f>1/(MIN($O$7/2,$P$7))^2</f>
-        <v>3265.3061224489634</v>
+        <v>1111.1111111111134</v>
       </c>
       <c r="I16">
         <f>SUM(Q7:Q11)</f>
@@ -927,11 +992,121 @@
       </c>
       <c r="J16">
         <f>SUM(R7:R11)</f>
-        <v>113.8888888888889</v>
+        <v>169.44444444444449</v>
       </c>
       <c r="K16">
         <f>SUM(S7:S11)</f>
         <v>100.00000000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F21">
+        <f>(1/F7) - 1</f>
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <f t="shared" ref="G21:J21" si="8">(1/G7) - 1</f>
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="8"/>
+        <v>0.4285714285714286</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="8"/>
+        <v>0.4285714285714286</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="8"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="22" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F22" s="9">
+        <f t="shared" ref="F22:J25" si="9">(1/F8) - 1</f>
+        <v>1</v>
+      </c>
+      <c r="G22" s="10">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="9"/>
+        <v>0.4285714285714286</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="9"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="23" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F23">
+        <f t="shared" si="9"/>
+        <v>5.666666666666667</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="9"/>
+        <v>0.4285714285714286</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="9"/>
+        <v>0.25</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="9"/>
+        <v>0.11111111111111116</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="9"/>
+        <v>0.11111111111111116</v>
+      </c>
+    </row>
+    <row r="24" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F24">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="9"/>
+        <v>0.4285714285714286</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="9"/>
+        <v>0.11111111111111116</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="9"/>
+        <v>0.11111111111111116</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="9"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="25" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F25">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="9"/>
+        <v>0.11111111111111116</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="9"/>
+        <v>0.11111111111111116</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="9"/>
+        <v>0.25</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="9"/>
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>
@@ -941,356 +1116,359 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7035605F-C406-4F9C-84F9-282F51FC6EEE}">
-  <dimension ref="D3:S16"/>
+  <dimension ref="D3:S25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15:K16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.1796875" customWidth="1"/>
-    <col min="16" max="16" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.21875" customWidth="1"/>
+    <col min="16" max="16" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="4:19" x14ac:dyDescent="0.3">
       <c r="E3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="4:19" x14ac:dyDescent="0.35">
-      <c r="E6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="8" t="s">
+      <c r="L3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="E6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="L6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="8" t="s">
+      <c r="M6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="N6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="O6" s="8" t="s">
+      <c r="O6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="P6" s="8" t="s">
+      <c r="P6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="Q6" s="8" t="s">
+      <c r="Q6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R6" s="8" t="s">
+      <c r="R6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="S6" s="9" t="s">
+      <c r="S6" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="4:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>1</v>
       </c>
-      <c r="F7" s="1">
-        <v>0.31</v>
-      </c>
-      <c r="G7" s="1">
+      <c r="F7" s="16">
+        <v>0.35</v>
+      </c>
+      <c r="G7" s="11">
         <v>0.6</v>
       </c>
-      <c r="H7" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="I7" s="1">
+      <c r="H7" s="11">
+        <v>0.7</v>
+      </c>
+      <c r="I7" s="11">
         <v>0.6</v>
       </c>
-      <c r="J7" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="K7" s="1">
+      <c r="J7" s="11">
+        <v>0.7</v>
+      </c>
+      <c r="K7" s="13">
         <f>SUM(F7:J7)/5</f>
-        <v>0.48199999999999993</v>
-      </c>
-      <c r="L7" s="1">
+        <v>0.59000000000000008</v>
+      </c>
+      <c r="L7">
         <v>0.3</v>
       </c>
-      <c r="M7" s="1" t="b">
+      <c r="M7" t="b">
         <f>MIN(F7:J7)&gt;L7</f>
         <v>1</v>
       </c>
-      <c r="N7" s="1" t="b">
+      <c r="N7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="O7" s="1">
-        <f>IF(OR($N$7:$N$11)=0,2,O10)</f>
-        <v>0.12400000000000008</v>
-      </c>
-      <c r="P7" s="1">
+      <c r="O7">
+        <f>IF(OR($N$7:$N$11)=0,2,O8)</f>
+        <v>0.11500000000000005</v>
+      </c>
+      <c r="P7">
         <f>ABS(MIN(F7:J7)-L7)</f>
-        <v>1.0000000000000009E-2</v>
-      </c>
-      <c r="Q7" s="1">
+        <v>4.9999999999999989E-2</v>
+      </c>
+      <c r="Q7">
         <f>(M7*N7/O7)^2</f>
         <v>0</v>
       </c>
-      <c r="R7" s="1">
+      <c r="R7">
         <f>((1-M7)*(1-N7)/P7)^2</f>
         <v>0</v>
       </c>
-      <c r="S7" s="3">
+      <c r="S7" s="2">
         <f>((1-M7)*N7/MAX(O7/2, P7))^2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="4:19" x14ac:dyDescent="0.35">
-      <c r="E8" s="5">
+    <row r="8" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="4">
         <v>2</v>
       </c>
-      <c r="F8" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="G8" s="1">
+      <c r="F8" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="G8" s="11">
         <v>0.2</v>
       </c>
-      <c r="H8" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="I8" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="J8" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="K8" s="1">
+      <c r="H8" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="I8" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="J8" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="K8" s="14">
         <f t="shared" ref="K8:K11" si="0">SUM(F8:J8)/5</f>
-        <v>0.54</v>
-      </c>
-      <c r="L8" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="L8">
         <v>0.3</v>
       </c>
-      <c r="M8" s="1" t="b">
+      <c r="M8" t="b">
         <f t="shared" ref="M8:M11" si="1">MIN(F8:J8)&gt;L8</f>
         <v>0</v>
       </c>
-      <c r="N8" s="1" t="b">
+      <c r="N8" t="b">
         <f>K8&lt;$K$7</f>
-        <v>0</v>
-      </c>
-      <c r="O8" s="1">
+        <v>1</v>
+      </c>
+      <c r="O8">
         <f>ABS(K8-$K$7)/2</f>
-        <v>2.9000000000000054E-2</v>
-      </c>
-      <c r="P8" s="1">
+        <v>0.11500000000000005</v>
+      </c>
+      <c r="P8">
         <f t="shared" ref="P8:P11" si="2">ABS(MIN(F8:J8)-L8)</f>
         <v>9.9999999999999978E-2</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="Q8">
         <f t="shared" ref="Q8:Q11" si="3">(M8*N8/O8)^2</f>
         <v>0</v>
       </c>
-      <c r="R8" s="1">
+      <c r="R8">
         <f t="shared" ref="R8:R11" si="4">((1-M8)*(1-N8)/P8)^2</f>
+        <v>0</v>
+      </c>
+      <c r="S8" s="2">
+        <f t="shared" ref="S8:S11" si="5">((1-M8)*N8/MAX(O8/2, P8))^2</f>
         <v>100.00000000000003</v>
       </c>
-      <c r="S8" s="3">
-        <f t="shared" ref="S8:S11" si="5">((1-M8)*N8/MAX(O8/2, P8))^2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="4:19" x14ac:dyDescent="0.35">
-      <c r="E9" s="5">
+    </row>
+    <row r="9" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="E9" s="4">
         <v>3</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="11">
         <v>0.15</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="11">
         <v>0.7</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="11">
         <v>0.8</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="11">
         <v>0.9</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="11">
         <v>0.9</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="14">
         <f t="shared" si="0"/>
         <v>0.69</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9">
         <v>0.3</v>
       </c>
-      <c r="M9" s="1" t="b">
+      <c r="M9" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N9" s="1" t="b">
+      <c r="N9" t="b">
         <f t="shared" ref="N9:N11" si="6">K9&lt;$K$7</f>
         <v>0</v>
       </c>
-      <c r="O9" s="1">
+      <c r="O9">
         <f t="shared" ref="O9:O11" si="7">ABS(K9-$K$7)/2</f>
-        <v>0.10400000000000001</v>
-      </c>
-      <c r="P9" s="1">
+        <v>4.9999999999999933E-2</v>
+      </c>
+      <c r="P9">
         <f t="shared" si="2"/>
         <v>0.15</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="Q9">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R9" s="1">
+      <c r="R9">
         <f t="shared" si="4"/>
         <v>44.44444444444445</v>
       </c>
-      <c r="S9" s="3">
+      <c r="S9" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="4:19" x14ac:dyDescent="0.35">
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="5">
+    <row r="10" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="E10" s="4">
         <v>4</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="11">
         <v>0.15</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="11">
         <v>0.9</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="11">
         <v>0.9</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="11">
         <v>0.9</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="11">
         <v>0.8</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="14">
         <f t="shared" si="0"/>
         <v>0.73000000000000009</v>
       </c>
-      <c r="L10" s="1">
+      <c r="L10">
         <v>0.3</v>
       </c>
-      <c r="M10" s="1" t="b">
+      <c r="M10" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N10" s="1" t="b">
+      <c r="N10" t="b">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O10" s="1">
+      <c r="O10">
         <f t="shared" si="7"/>
-        <v>0.12400000000000008</v>
-      </c>
-      <c r="P10" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="P10">
         <f t="shared" si="2"/>
         <v>0.15</v>
       </c>
-      <c r="Q10" s="1">
+      <c r="Q10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R10" s="1">
+      <c r="R10">
         <f t="shared" si="4"/>
         <v>44.44444444444445</v>
       </c>
-      <c r="S10" s="3">
+      <c r="S10" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="4:19" x14ac:dyDescent="0.35">
-      <c r="E11" s="6">
+    <row r="11" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="E11" s="5">
         <v>5</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="12">
         <v>0.1</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="12">
         <v>0.9</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="12">
         <v>0.9</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="12">
         <v>0.8</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="12">
         <v>0.8</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="15">
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11" s="1">
         <v>0.3</v>
       </c>
-      <c r="M11" s="2" t="b">
+      <c r="M11" s="1" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N11" s="2" t="b">
+      <c r="N11" s="1" t="b">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O11" s="2">
+      <c r="O11" s="1">
         <f t="shared" si="7"/>
-        <v>0.10900000000000001</v>
-      </c>
-      <c r="P11" s="2">
+        <v>5.4999999999999938E-2</v>
+      </c>
+      <c r="P11" s="1">
         <f t="shared" si="2"/>
         <v>0.19999999999999998</v>
       </c>
-      <c r="Q11" s="2">
+      <c r="Q11" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R11" s="2">
+      <c r="R11" s="1">
         <f t="shared" si="4"/>
         <v>25</v>
       </c>
-      <c r="S11" s="4">
+      <c r="S11" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="4:19" x14ac:dyDescent="0.35">
+    <row r="15" spans="4:19" x14ac:dyDescent="0.3">
       <c r="H15" t="s">
         <v>8</v>
       </c>
@@ -1304,10 +1482,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="4:19" x14ac:dyDescent="0.35">
+    <row r="16" spans="4:19" x14ac:dyDescent="0.3">
       <c r="H16">
         <f>1/(MIN($O$7/2,$P$7))^2</f>
-        <v>9999.9999999999818</v>
+        <v>400.00000000000023</v>
       </c>
       <c r="I16">
         <f>SUM(Q7:Q11)</f>
@@ -1315,11 +1493,121 @@
       </c>
       <c r="J16">
         <f>SUM(R7:R11)</f>
-        <v>213.88888888888894</v>
+        <v>113.8888888888889</v>
       </c>
       <c r="K16">
         <f>SUM(S7:S11)</f>
-        <v>0</v>
+        <v>100.00000000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F21" s="9">
+        <f>(1/F7) - 1</f>
+        <v>1.8571428571428572</v>
+      </c>
+      <c r="G21">
+        <f t="shared" ref="G21:J21" si="8">(1/G7) - 1</f>
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="8"/>
+        <v>0.4285714285714286</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="8"/>
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="8"/>
+        <v>0.4285714285714286</v>
+      </c>
+    </row>
+    <row r="22" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F22">
+        <f t="shared" ref="F22:J25" si="9">(1/F8) - 1</f>
+        <v>1.5</v>
+      </c>
+      <c r="G22" s="10">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="9"/>
+        <v>1.5</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="9"/>
+        <v>1.5</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="9"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="23" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F23">
+        <f t="shared" si="9"/>
+        <v>5.666666666666667</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="9"/>
+        <v>0.4285714285714286</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="9"/>
+        <v>0.25</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="9"/>
+        <v>0.11111111111111116</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="9"/>
+        <v>0.11111111111111116</v>
+      </c>
+    </row>
+    <row r="24" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F24">
+        <f t="shared" si="9"/>
+        <v>5.666666666666667</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="9"/>
+        <v>0.11111111111111116</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="9"/>
+        <v>0.11111111111111116</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="9"/>
+        <v>0.11111111111111116</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="9"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="25" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F25">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="9"/>
+        <v>0.11111111111111116</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="9"/>
+        <v>0.11111111111111116</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="9"/>
+        <v>0.25</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="9"/>
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>
@@ -1329,348 +1617,348 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE98EAC6-D89C-4191-BCB3-855D45FA60EC}">
-  <dimension ref="D3:S16"/>
+  <dimension ref="D3:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="4:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="4:19" x14ac:dyDescent="0.3">
       <c r="E3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="4:19" x14ac:dyDescent="0.35">
-      <c r="E6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="8" t="s">
+    <row r="6" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="E6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="L6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="8" t="s">
+      <c r="M6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="N6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="O6" s="8" t="s">
+      <c r="O6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="P6" s="8" t="s">
+      <c r="P6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="Q6" s="8" t="s">
+      <c r="Q6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R6" s="8" t="s">
+      <c r="R6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="S6" s="9" t="s">
+      <c r="S6" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="4:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>1</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="11">
         <v>0.7</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="11">
         <v>0.6</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="11">
         <v>0.8</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="11">
         <v>0.7</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="11">
         <v>0.9</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="13">
         <f>SUM(F7:J7)/5</f>
         <v>0.74</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7">
         <v>0.3</v>
       </c>
-      <c r="M7" s="1" t="b">
+      <c r="M7" t="b">
         <f>MIN(F7:J7)&gt;L7</f>
         <v>1</v>
       </c>
-      <c r="N7" s="1" t="b">
+      <c r="N7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="O7" s="1">
+      <c r="O7">
         <f>IF(OR($N$7:$N$11)=0,2,O10)</f>
         <v>4.9999999999999489E-3</v>
       </c>
-      <c r="P7" s="1">
+      <c r="P7">
         <f>ABS(MIN(F7:J7)-L7)</f>
         <v>0.3</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="Q7">
         <f>(M7*N7/O7)^2</f>
         <v>0</v>
       </c>
-      <c r="R7" s="1">
+      <c r="R7">
         <f>((1-M7)*(1-N7)/P7)^2</f>
         <v>0</v>
       </c>
-      <c r="S7" s="3">
+      <c r="S7" s="2">
         <f>((1-M7)*N7/MAX(O7/2, P7))^2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="4:19" x14ac:dyDescent="0.35">
-      <c r="E8" s="5">
+    <row r="8" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="E8" s="4">
         <v>2</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="11">
         <v>0.7</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="H8" s="11">
         <v>0.7</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="11">
         <v>0.7</v>
       </c>
-      <c r="I8" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="J8" s="1">
+      <c r="J8" s="11">
         <v>0.8</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="14">
         <f t="shared" ref="K8:K11" si="0">SUM(F8:J8)/5</f>
-        <v>0.72</v>
-      </c>
-      <c r="L8" s="1">
+        <v>0.67999999999999994</v>
+      </c>
+      <c r="L8">
         <v>0.3</v>
       </c>
-      <c r="M8" s="1" t="b">
+      <c r="M8" t="b">
         <f t="shared" ref="M8:M11" si="1">MIN(F8:J8)&gt;L8</f>
         <v>1</v>
       </c>
-      <c r="N8" s="1" t="b">
+      <c r="N8" t="b">
         <f>K8&lt;$K$7</f>
         <v>1</v>
       </c>
-      <c r="O8" s="1">
+      <c r="O8">
         <f>ABS(K8-$K$7)/2</f>
-        <v>1.0000000000000009E-2</v>
-      </c>
-      <c r="P8" s="1">
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="P8">
         <f t="shared" ref="P8:P11" si="2">ABS(MIN(F8:J8)-L8)</f>
-        <v>0.39999999999999997</v>
-      </c>
-      <c r="Q8" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="Q8">
         <f t="shared" ref="Q8:Q11" si="3">(M8*N8/O8)^2</f>
-        <v>9999.9999999999836</v>
-      </c>
-      <c r="R8" s="1">
+        <v>1111.1111111111088</v>
+      </c>
+      <c r="R8">
         <f t="shared" ref="R8:R11" si="4">((1-M8)*(1-N8)/P8)^2</f>
         <v>0</v>
       </c>
-      <c r="S8" s="3">
+      <c r="S8" s="2">
         <f t="shared" ref="S8:S11" si="5">((1-M8)*N8/MAX(O8/2, P8))^2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="4:19" x14ac:dyDescent="0.35">
-      <c r="E9" s="5">
+    <row r="9" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="E9" s="4">
         <v>3</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="11">
         <v>0.15</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="11">
         <v>0.7</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="11">
         <v>0.8</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="11">
         <v>0.9</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="11">
         <v>0.9</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="14">
         <f t="shared" si="0"/>
         <v>0.69</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9">
         <v>0.3</v>
       </c>
-      <c r="M9" s="1" t="b">
+      <c r="M9" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N9" s="1" t="b">
+      <c r="N9" t="b">
         <f t="shared" ref="N9:N11" si="6">K9&lt;$K$7</f>
         <v>1</v>
       </c>
-      <c r="O9" s="1">
+      <c r="O9">
         <f t="shared" ref="O9:O11" si="7">ABS(K9-$K$7)/2</f>
         <v>2.5000000000000022E-2</v>
       </c>
-      <c r="P9" s="1">
+      <c r="P9">
         <f t="shared" si="2"/>
         <v>0.15</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="Q9">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R9" s="1">
+      <c r="R9">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="S9" s="3">
+      <c r="S9" s="2">
         <f t="shared" si="5"/>
         <v>44.44444444444445</v>
       </c>
     </row>
-    <row r="10" spans="4:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>4</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="11">
         <v>0.15</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="11">
         <v>0.9</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="11">
         <v>0.9</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="11">
         <v>0.9</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="11">
         <v>0.8</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="14">
         <f t="shared" si="0"/>
         <v>0.73000000000000009</v>
       </c>
-      <c r="L10" s="1">
+      <c r="L10">
         <v>0.3</v>
       </c>
-      <c r="M10" s="1" t="b">
+      <c r="M10" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N10" s="1" t="b">
+      <c r="N10" t="b">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="O10" s="1">
+      <c r="O10">
         <f t="shared" si="7"/>
         <v>4.9999999999999489E-3</v>
       </c>
-      <c r="P10" s="1">
+      <c r="P10">
         <f t="shared" si="2"/>
         <v>0.15</v>
       </c>
-      <c r="Q10" s="1">
+      <c r="Q10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R10" s="1">
+      <c r="R10">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="S10" s="3">
+      <c r="S10" s="2">
         <f t="shared" si="5"/>
         <v>44.44444444444445</v>
       </c>
     </row>
-    <row r="11" spans="4:19" x14ac:dyDescent="0.35">
-      <c r="E11" s="6">
+    <row r="11" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="E11" s="5">
         <v>5</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="12">
         <v>0.1</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="12">
         <v>0.9</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="12">
         <v>0.9</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="12">
         <v>0.8</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="12">
         <v>0.8</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="15">
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11" s="1">
         <v>0.3</v>
       </c>
-      <c r="M11" s="2" t="b">
+      <c r="M11" s="1" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N11" s="2" t="b">
+      <c r="N11" s="1" t="b">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="O11" s="2">
+      <c r="O11" s="1">
         <f t="shared" si="7"/>
         <v>2.0000000000000018E-2</v>
       </c>
-      <c r="P11" s="2">
+      <c r="P11" s="1">
         <f t="shared" si="2"/>
         <v>0.19999999999999998</v>
       </c>
-      <c r="Q11" s="2">
+      <c r="Q11" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R11" s="2">
+      <c r="R11" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="S11" s="4">
+      <c r="S11" s="3">
         <f t="shared" si="5"/>
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="4:19" x14ac:dyDescent="0.35">
+    <row r="15" spans="4:19" x14ac:dyDescent="0.3">
       <c r="H15" t="s">
         <v>8</v>
       </c>
@@ -1684,14 +1972,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="4:19" x14ac:dyDescent="0.35">
+    <row r="16" spans="4:19" x14ac:dyDescent="0.3">
       <c r="H16">
         <f>1/(MIN($O$7/2,$P$7))^2</f>
         <v>160000.00000000326</v>
       </c>
       <c r="I16">
         <f>SUM(Q7:Q11)</f>
-        <v>9999.9999999999836</v>
+        <v>1111.1111111111088</v>
       </c>
       <c r="J16">
         <f>SUM(R7:R11)</f>
@@ -1700,6 +1988,116 @@
       <c r="K16">
         <f>SUM(S7:S11)</f>
         <v>113.8888888888889</v>
+      </c>
+    </row>
+    <row r="21" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F21">
+        <f>(1/F7) - 1</f>
+        <v>0.4285714285714286</v>
+      </c>
+      <c r="G21">
+        <f t="shared" ref="G21:J21" si="8">(1/G7) - 1</f>
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="8"/>
+        <v>0.25</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="8"/>
+        <v>0.4285714285714286</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="8"/>
+        <v>0.11111111111111116</v>
+      </c>
+    </row>
+    <row r="22" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F22">
+        <f t="shared" ref="F22:J22" si="9">(1/F8) - 1</f>
+        <v>0.4285714285714286</v>
+      </c>
+      <c r="G22" s="9">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="9"/>
+        <v>0.4285714285714286</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="9"/>
+        <v>0.4285714285714286</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="9"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="23" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F23">
+        <f t="shared" ref="F23:J23" si="10">(1/F9) - 1</f>
+        <v>5.666666666666667</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="10"/>
+        <v>0.4285714285714286</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="10"/>
+        <v>0.25</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="10"/>
+        <v>0.11111111111111116</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="10"/>
+        <v>0.11111111111111116</v>
+      </c>
+    </row>
+    <row r="24" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F24">
+        <f t="shared" ref="F24:J24" si="11">(1/F10) - 1</f>
+        <v>5.666666666666667</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="11"/>
+        <v>0.11111111111111116</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="11"/>
+        <v>0.11111111111111116</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="11"/>
+        <v>0.11111111111111116</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="11"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="25" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F25">
+        <f t="shared" ref="F25:J25" si="12">(1/F11) - 1</f>
+        <v>9</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="12"/>
+        <v>0.11111111111111116</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="12"/>
+        <v>0.11111111111111116</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="12"/>
+        <v>0.25</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="12"/>
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>